<commit_message>
Changes to character list
</commit_message>
<xml_diff>
--- a/Character List.xlsx
+++ b/Character List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seinhuis\Dropbox\Google Drive\Splitflap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Splitflap_Display\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{905CE15C-ADEF-42FF-95CD-C638673CEE54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA30ED-109D-4E3C-AA9A-DAA8A3702F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A85C054D-02AD-4130-BFA1-B7A709620B49}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{A85C054D-02AD-4130-BFA1-B7A709620B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Character List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Character List'!$A$1:$H$50</definedName>
+    <definedName name="Print_Area" localSheetId="0">'Character List'!$A$1:$L$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Applies:</t>
   </si>
@@ -138,15 +141,6 @@
     <t>EXT</t>
   </si>
   <si>
-    <t>IR *</t>
-  </si>
-  <si>
-    <t>IT *</t>
-  </si>
-  <si>
-    <t>? *</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>Kruis **</t>
   </si>
   <si>
-    <t>Orient **</t>
-  </si>
-  <si>
     <t>Dienst **</t>
   </si>
   <si>
@@ -265,13 +256,25 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Width (mm)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Height (mm)</t>
+  </si>
+  <si>
+    <t>Dining **</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +310,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -316,7 +326,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -436,11 +446,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -489,20 +651,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,19 +1025,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection sqref="A1:L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -846,14 +1056,22 @@
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -866,14 +1084,22 @@
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="14">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="I2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="28">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L2" s="36">
+        <v>36.706000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -886,14 +1112,22 @@
       <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="14">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="I3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="28">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L3" s="36">
+        <v>34.582999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -906,14 +1140,22 @@
       <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="14">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="I4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="28">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L4" s="36">
+        <v>32.155999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -926,14 +1168,22 @@
       <c r="E5" s="6">
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="I5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="28">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L5" s="36">
+        <v>37.313000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -946,14 +1196,22 @@
       <c r="E6" s="6">
         <v>4</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="14">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="I6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="28">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L6" s="36">
+        <v>30.638999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -966,14 +1224,22 @@
       <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="14">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="I7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="28">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L7" s="36">
+        <v>28.617000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -986,88 +1252,128 @@
       <c r="E8" s="6">
         <v>6</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="I8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="28">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L8" s="36">
+        <v>37.414000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="6">
         <v>7</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="I9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="28">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L9" s="36">
+        <v>33.975999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="I10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="28">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L10" s="36">
+        <v>6.8760000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="6">
         <v>9</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="14">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="I11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="28">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="3" t="s">
+      <c r="K11" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L11" s="36">
+        <v>15.977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="6">
         <v>10</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="14">
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="I12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="28">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L12" s="36">
+        <v>34.177999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
@@ -1075,153 +1381,237 @@
         <v>3</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="E13" s="6">
         <v>11</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="I13" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="14">
+      <c r="J13" s="28">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L13" s="36">
+        <v>30.538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="7">
         <v>12</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="14">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="I14" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="28">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L14" s="36">
+        <v>37.616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="6">
-        <v>13</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="14">
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="I15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="28">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L15" s="36">
+        <v>33.47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="6">
-        <v>14</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="14">
+      <c r="D16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="28">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L16" s="36">
+        <v>38.021000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="6">
         <v>3</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="7">
-        <v>15</v>
-      </c>
-      <c r="G17" s="16" t="s">
+      <c r="D17" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="14">
+      <c r="J17" s="28">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L17" s="36">
+        <v>33.875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="6">
         <v>4</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="14">
+      <c r="D18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="28">
+        <v>1</v>
+      </c>
+      <c r="F18" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G18" s="36">
+        <v>36.706000000000003</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="28">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L18" s="36">
+        <v>38.222999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="6">
         <v>5</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="28">
+        <v>2</v>
+      </c>
+      <c r="F19" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G19" s="36">
+        <v>34.582999999999998</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="28">
         <v>48</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K19" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L19" s="36">
+        <v>33.268000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="6">
         <v>6</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="H20" s="14">
+      <c r="D20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="28">
+        <v>3</v>
+      </c>
+      <c r="F20" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G20" s="36">
+        <v>32.155999999999999</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="28">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K20" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L20" s="36">
+        <v>31.042999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -1229,19 +1619,31 @@
         <v>7</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="28">
+        <v>4</v>
+      </c>
+      <c r="F21" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G21" s="36">
+        <v>37.313000000000002</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="28">
         <v>50</v>
       </c>
-      <c r="E21" s="14">
-        <v>1</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L21" s="36">
+        <v>33.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1251,17 +1653,29 @@
       <c r="D22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="14">
-        <v>2</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="14">
+      <c r="E22" s="28">
+        <v>5</v>
+      </c>
+      <c r="F22" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G22" s="36">
+        <v>30.638999999999999</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="28">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K22" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L22" s="36">
+        <v>33.167000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -1269,19 +1683,31 @@
         <v>9</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="14">
-        <v>3</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="14">
+        <v>50</v>
+      </c>
+      <c r="E23" s="28">
+        <v>6</v>
+      </c>
+      <c r="F23" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G23" s="36">
+        <v>28.617000000000001</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="28">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L23" s="36">
+        <v>35.896999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1289,19 +1715,31 @@
         <v>10</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="14">
-        <v>4</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="14">
+        <v>51</v>
+      </c>
+      <c r="E24" s="28">
+        <v>7</v>
+      </c>
+      <c r="F24" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G24" s="36">
+        <v>37.414000000000001</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="28">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K24" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L24" s="36">
+        <v>38.930999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>14</v>
       </c>
@@ -1309,19 +1747,31 @@
         <v>11</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="14">
-        <v>5</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H25" s="14">
+        <v>52</v>
+      </c>
+      <c r="E25" s="28">
+        <v>8</v>
+      </c>
+      <c r="F25" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G25" s="36">
+        <v>33.975999999999999</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="28">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L25" s="36">
+        <v>34.177999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -1329,19 +1779,31 @@
         <v>12</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="14">
-        <v>6</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H26" s="14">
+        <v>53</v>
+      </c>
+      <c r="E26" s="28">
+        <v>9</v>
+      </c>
+      <c r="F26" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G26" s="36">
+        <v>6.8760000000000003</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="28">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K26" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L26" s="36">
+        <v>35.493000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -1349,19 +1811,31 @@
         <v>13</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="14">
-        <v>7</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="H27" s="14">
+        <v>54</v>
+      </c>
+      <c r="E27" s="28">
+        <v>10</v>
+      </c>
+      <c r="F27" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G27" s="36">
+        <v>15.977</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="28">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K27" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L27" s="36">
+        <v>33.975999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -1369,19 +1843,31 @@
         <v>14</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="14">
-        <v>8</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="14">
+        <v>55</v>
+      </c>
+      <c r="E28" s="28">
+        <v>11</v>
+      </c>
+      <c r="F28" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G28" s="36">
+        <v>34.177999999999997</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="28">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K28" s="28">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="L28" s="14">
+        <v>37.716999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
@@ -1389,19 +1875,31 @@
         <v>15</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="14">
-        <v>9</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="14">
+        <v>31</v>
+      </c>
+      <c r="E29" s="28">
+        <v>12</v>
+      </c>
+      <c r="F29" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G29" s="36">
+        <v>30.538</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="28">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="35">
+        <v>6.3230000000000004</v>
+      </c>
+      <c r="L29" s="36">
+        <v>34.279000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>19</v>
       </c>
@@ -1409,19 +1907,31 @@
         <v>16</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="14">
-        <v>10</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H30" s="18">
+        <v>56</v>
+      </c>
+      <c r="E30" s="28">
+        <v>13</v>
+      </c>
+      <c r="F30" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G30" s="36">
+        <v>37.616</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="29">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="37">
+        <v>6.6280000000000001</v>
+      </c>
+      <c r="L30" s="38">
+        <v>15.571999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>20</v>
       </c>
@@ -1429,15 +1939,23 @@
         <v>17</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="14">
-        <v>11</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E31" s="28">
+        <v>14</v>
+      </c>
+      <c r="F31" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G31" s="36">
+        <v>33.47</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1445,19 +1963,25 @@
         <v>18</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="14">
-        <v>12</v>
-      </c>
-      <c r="G32" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E32" s="28">
+        <v>15</v>
+      </c>
+      <c r="F32" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G32" s="36">
+        <v>38.021000000000001</v>
+      </c>
+      <c r="I32" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
@@ -1465,19 +1989,25 @@
         <v>19</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="14">
-        <v>13</v>
-      </c>
-      <c r="G33" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E33" s="28">
+        <v>16</v>
+      </c>
+      <c r="F33" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G33" s="36">
+        <v>33.875</v>
+      </c>
+      <c r="I33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>23</v>
       </c>
@@ -1485,13 +2015,19 @@
         <v>20</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E34" s="28">
+        <v>17</v>
+      </c>
+      <c r="F34" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G34" s="36">
+        <v>38.222999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>24</v>
       </c>
@@ -1499,13 +2035,19 @@
         <v>21</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E35" s="28">
+        <v>18</v>
+      </c>
+      <c r="F35" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G35" s="36">
+        <v>33.268000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -1513,13 +2055,19 @@
         <v>22</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E36" s="28">
+        <v>19</v>
+      </c>
+      <c r="F36" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G36" s="36">
+        <v>31.042999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>26</v>
       </c>
@@ -1527,13 +2075,19 @@
         <v>23</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="14">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E37" s="28">
+        <v>20</v>
+      </c>
+      <c r="F37" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G37" s="36">
+        <v>33.47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
@@ -1541,115 +2095,151 @@
         <v>24</v>
       </c>
       <c r="D38" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="28">
+        <v>21</v>
+      </c>
+      <c r="F38" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G38" s="36">
+        <v>33.167000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="28">
+        <v>22</v>
+      </c>
+      <c r="F39" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G39" s="36">
+        <v>35.896999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="15" t="s">
+      <c r="E40" s="28">
+        <v>23</v>
+      </c>
+      <c r="F40" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G40" s="36">
+        <v>38.930999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="14">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="15" t="s">
+      <c r="E41" s="28">
+        <v>24</v>
+      </c>
+      <c r="F41" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G41" s="36">
+        <v>34.177999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="14">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="15" t="s">
+      <c r="E42" s="28">
+        <v>25</v>
+      </c>
+      <c r="F42" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G42" s="36">
+        <v>35.493000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D43" s="15" t="s">
+      <c r="E43" s="28">
+        <v>26</v>
+      </c>
+      <c r="F43" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G43" s="36">
+        <v>33.975999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="15" t="s">
+      <c r="E44" s="28">
+        <v>27</v>
+      </c>
+      <c r="F44" s="35">
+        <v>6.3230000000000004</v>
+      </c>
+      <c r="G44" s="36">
+        <v>34.279000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="14">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="15" t="s">
+      <c r="E45" s="28">
+        <v>28</v>
+      </c>
+      <c r="F45" s="35">
+        <v>6.6280000000000001</v>
+      </c>
+      <c r="G45" s="36">
+        <v>15.571999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="14">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="14">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D48" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" s="14">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="15" t="s">
+      <c r="E46" s="28">
+        <v>29</v>
+      </c>
+      <c r="F46" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G46" s="36">
+        <v>25.684000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="23">
+        <v>30</v>
+      </c>
+      <c r="F47" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E49" s="14">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="4:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G47" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="12"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
General changes for mental wellbeing
</commit_message>
<xml_diff>
--- a/Character List.xlsx
+++ b/Character List.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Splitflap_Display\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA30ED-109D-4E3C-AA9A-DAA8A3702F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABA5661-8433-4CA8-A1B7-5F6D60DBCB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{A85C054D-02AD-4130-BFA1-B7A709620B49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A85C054D-02AD-4130-BFA1-B7A709620B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Character List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Area" localSheetId="0">'Character List'!$A$1:$L$47</definedName>
+    <definedName name="Lijst" localSheetId="0">'Character List'!$A$1:$L$47</definedName>
+    <definedName name="Print_Area" localSheetId="0">'Character List'!$A$1:$L$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
   <si>
     <t>Applies:</t>
   </si>
@@ -153,9 +154,6 @@
     <t>MW **</t>
   </si>
   <si>
-    <t>Kruis **</t>
-  </si>
-  <si>
     <t>Dienst **</t>
   </si>
   <si>
@@ -268,6 +266,18 @@
   </si>
   <si>
     <t>Dining **</t>
+  </si>
+  <si>
+    <t>Sint**</t>
+  </si>
+  <si>
+    <t>Event**</t>
+  </si>
+  <si>
+    <t>Diesel **</t>
+  </si>
+  <si>
+    <t>Groep **</t>
   </si>
 </sst>
 </file>
@@ -1027,12 +1037,13 @@
   </sheetPr>
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L47"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection sqref="A1:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -1062,13 +1073,13 @@
         <v>0</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1087,7 +1098,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="I2" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="28">
         <v>31</v>
@@ -1115,7 +1126,7 @@
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
       <c r="I3" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J3" s="28">
         <v>32</v>
@@ -1143,7 +1154,7 @@
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
       <c r="I4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" s="28">
         <v>33</v>
@@ -1171,7 +1182,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="I5" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" s="28">
         <v>34</v>
@@ -1199,7 +1210,7 @@
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="I6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" s="28">
         <v>35</v>
@@ -1227,7 +1238,7 @@
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="I7" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" s="28">
         <v>36</v>
@@ -1255,7 +1266,7 @@
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="I8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" s="28">
         <v>37</v>
@@ -1283,7 +1294,7 @@
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="I9" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" s="28">
         <v>38</v>
@@ -1311,7 +1322,7 @@
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="I10" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J10" s="28">
         <v>39</v>
@@ -1331,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="E11" s="6">
         <v>9</v>
@@ -1339,7 +1350,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="I11" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" s="28">
         <v>40</v>
@@ -1352,8 +1363,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="10" t="s">
-        <v>38</v>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="6">
         <v>10</v>
@@ -1361,7 +1372,7 @@
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="I12" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J12" s="28">
         <v>41</v>
@@ -1380,10 +1391,10 @@
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="14">
         <v>11</v>
       </c>
       <c r="F13" s="22"/>
@@ -1401,23 +1412,23 @@
         <v>30.538</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="14">
         <v>12</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="I14" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J14" s="28">
         <v>43</v>
@@ -1429,17 +1440,23 @@
         <v>37.616</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="6">
+        <v>13</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="I15" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J15" s="28">
         <v>44</v>
@@ -1451,27 +1468,21 @@
         <v>33.47</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="D16" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="25" t="s">
-        <v>73</v>
+      <c r="E16" s="6">
+        <v>14</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="28">
         <v>45</v>
@@ -1483,24 +1494,18 @@
         <v>38.021000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="6">
         <v>3</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="24">
-        <v>0</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>74</v>
+      <c r="D17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="7">
+        <v>15</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>32</v>
@@ -1515,27 +1520,15 @@
         <v>33.875</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="6">
         <v>4</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="28">
-        <v>1</v>
-      </c>
-      <c r="F18" s="35">
-        <v>36.712000000000003</v>
-      </c>
-      <c r="G18" s="36">
-        <v>36.706000000000003</v>
-      </c>
       <c r="I18" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J18" s="28">
         <v>47</v>
@@ -1547,27 +1540,27 @@
         <v>38.222999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="6">
         <v>5</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="28">
-        <v>2</v>
-      </c>
-      <c r="F19" s="35">
-        <v>36.712000000000003</v>
-      </c>
-      <c r="G19" s="36">
-        <v>34.582999999999998</v>
+      <c r="D19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="28">
         <v>48</v>
@@ -1586,20 +1579,20 @@
       <c r="B20" s="6">
         <v>6</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="28">
-        <v>3</v>
-      </c>
-      <c r="F20" s="35">
-        <v>36.712000000000003</v>
-      </c>
-      <c r="G20" s="36">
-        <v>32.155999999999999</v>
+      <c r="D20" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J20" s="28">
         <v>49</v>
@@ -1619,16 +1612,16 @@
         <v>7</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E21" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G21" s="36">
-        <v>37.313000000000002</v>
+        <v>36.706000000000003</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>35</v>
@@ -1651,19 +1644,19 @@
         <v>8</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E22" s="28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F22" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G22" s="36">
-        <v>30.638999999999999</v>
+        <v>34.582999999999998</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J22" s="28">
         <v>51</v>
@@ -1683,19 +1676,19 @@
         <v>9</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E23" s="28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F23" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G23" s="36">
-        <v>28.617000000000001</v>
+        <v>32.155999999999999</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" s="28">
         <v>52</v>
@@ -1715,19 +1708,19 @@
         <v>10</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" s="28">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F24" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G24" s="36">
-        <v>37.414000000000001</v>
+        <v>37.313000000000002</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J24" s="28">
         <v>53</v>
@@ -1747,19 +1740,19 @@
         <v>11</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" s="28">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F25" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G25" s="36">
-        <v>33.975999999999999</v>
+        <v>30.638999999999999</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J25" s="28">
         <v>54</v>
@@ -1779,19 +1772,19 @@
         <v>12</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E26" s="28">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F26" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G26" s="36">
-        <v>6.8760000000000003</v>
+        <v>28.617000000000001</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J26" s="28">
         <v>55</v>
@@ -1811,19 +1804,19 @@
         <v>13</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E27" s="28">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F27" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G27" s="36">
-        <v>15.977</v>
+        <v>37.414000000000001</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="28">
         <v>56</v>
@@ -1843,19 +1836,19 @@
         <v>14</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E28" s="28">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F28" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G28" s="36">
-        <v>34.177999999999997</v>
+        <v>33.975999999999999</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J28" s="28">
         <v>57</v>
@@ -1875,19 +1868,19 @@
         <v>15</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E29" s="28">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G29" s="36">
-        <v>30.538</v>
+        <v>6.8760000000000003</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J29" s="28">
         <v>58</v>
@@ -1907,19 +1900,19 @@
         <v>16</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E30" s="28">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F30" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G30" s="36">
-        <v>37.616</v>
+        <v>15.977</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J30" s="29">
         <v>59</v>
@@ -1939,16 +1932,16 @@
         <v>17</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E31" s="28">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F31" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G31" s="36">
-        <v>33.47</v>
+        <v>34.177999999999997</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="13"/>
@@ -1963,22 +1956,22 @@
         <v>18</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E32" s="28">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F32" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G32" s="36">
-        <v>38.021000000000001</v>
+        <v>30.538</v>
       </c>
       <c r="I32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1989,22 +1982,22 @@
         <v>19</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E33" s="28">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F33" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G33" s="36">
-        <v>33.875</v>
+        <v>37.616</v>
       </c>
       <c r="I33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2015,16 +2008,16 @@
         <v>20</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E34" s="28">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F34" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G34" s="36">
-        <v>38.222999999999999</v>
+        <v>33.47</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2035,16 +2028,16 @@
         <v>21</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E35" s="28">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F35" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G35" s="36">
-        <v>33.268000000000001</v>
+        <v>38.021000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2055,16 +2048,16 @@
         <v>22</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E36" s="28">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F36" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G36" s="36">
-        <v>31.042999999999999</v>
+        <v>33.875</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2075,16 +2068,16 @@
         <v>23</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E37" s="28">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F37" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G37" s="36">
-        <v>33.47</v>
+        <v>38.222999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2095,145 +2088,187 @@
         <v>24</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E38" s="28">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F38" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G38" s="36">
-        <v>33.167000000000002</v>
+        <v>33.268000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D39" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E39" s="28">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F39" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G39" s="36">
-        <v>35.896999999999998</v>
+        <v>31.042999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D40" s="15" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E40" s="28">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F40" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G40" s="36">
-        <v>38.930999999999997</v>
+        <v>33.47</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D41" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E41" s="28">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F41" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G41" s="36">
-        <v>34.177999999999997</v>
+        <v>33.167000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D42" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E42" s="28">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F42" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G42" s="36">
-        <v>35.493000000000002</v>
+        <v>35.896999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D43" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E43" s="28">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F43" s="35">
         <v>36.712000000000003</v>
       </c>
       <c r="G43" s="36">
-        <v>33.975999999999999</v>
+        <v>38.930999999999997</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E44" s="28">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F44" s="35">
-        <v>6.3230000000000004</v>
+        <v>36.712000000000003</v>
       </c>
       <c r="G44" s="36">
-        <v>34.279000000000003</v>
+        <v>34.177999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D45" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E45" s="28">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F45" s="35">
-        <v>6.6280000000000001</v>
+        <v>36.712000000000003</v>
       </c>
       <c r="G45" s="36">
-        <v>15.571999999999999</v>
+        <v>35.493000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D46" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E46" s="28">
+        <v>26</v>
+      </c>
+      <c r="F46" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G46" s="36">
+        <v>33.975999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="28">
+        <v>27</v>
+      </c>
+      <c r="F47" s="35">
+        <v>6.3230000000000004</v>
+      </c>
+      <c r="G47" s="36">
+        <v>34.279000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="28">
+        <v>28</v>
+      </c>
+      <c r="F48" s="35">
+        <v>6.6280000000000001</v>
+      </c>
+      <c r="G48" s="36">
+        <v>15.571999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="28">
         <v>29</v>
       </c>
-      <c r="F46" s="35">
-        <v>36.712000000000003</v>
-      </c>
-      <c r="G46" s="36">
+      <c r="F49" s="35">
+        <v>36.712000000000003</v>
+      </c>
+      <c r="G49" s="36">
         <v>25.684000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="20" t="s">
+    <row r="50" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="23">
+      <c r="E50" s="23">
         <v>30</v>
       </c>
-      <c r="F47" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="G47" s="34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F50" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G50" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="12"/>
     </row>

</xml_diff>